<commit_message>
Dashborad e 2 relatórios feitos
Só falta a manutenção
</commit_message>
<xml_diff>
--- a/Perg3/Dados.xlsx
+++ b/Perg3/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\CM\CMO\Perg3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52957B33-5F3A-4F3D-90F5-B868D3D9FC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B0FD3-0E1A-4DCA-AC71-12F04BF81F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23118" yWindow="0" windowWidth="20886" windowHeight="12318" xr2:uid="{7EB9C257-8B1E-47F7-B951-8690B91EF030}"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="27570" windowHeight="15120" xr2:uid="{7EB9C257-8B1E-47F7-B951-8690B91EF030}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Saúde</t>
   </si>
   <si>
-    <t>Carro</t>
-  </si>
-  <si>
     <t>Satus</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Valor segurado</t>
+  </si>
+  <si>
+    <t>Automóvel</t>
   </si>
 </sst>
 </file>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BED1EA-2019-4850-8E9E-3498337B34DC}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -555,7 +555,7 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -766,13 +766,13 @@
         <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M8">
         <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -832,9 +832,6 @@
       <c r="I10">
         <v>36000</v>
       </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -864,88 +861,153 @@
       <c r="I11">
         <v>44000</v>
       </c>
-      <c r="K11" t="s">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>125</v>
+      </c>
+      <c r="I12">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>650</v>
+      </c>
+      <c r="I13">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
         <v>22</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K13">
-        <v>2</v>
-      </c>
-      <c r="L13" t="s">
+    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14" t="s">
+    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K15">
-        <v>4</v>
-      </c>
-      <c r="L15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
-        <v>5</v>
-      </c>
-      <c r="L18" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20" t="s">
+    <row r="24" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K21">
-        <v>3</v>
-      </c>
-      <c r="L21" t="s">
+    <row r="25" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K22">
-        <v>4</v>
-      </c>
-      <c r="L22" t="s">
-        <v>32</v>
+    <row r="26" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>